<commit_message>
Updated 1M resistors to 2M based on component availability
</commit_message>
<xml_diff>
--- a/BatteryBoard/bom/bom_pcb.xlsx
+++ b/BatteryBoard/bom/bom_pcb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="21600" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom_pcb" sheetId="1" r:id="rId1"/>
@@ -544,13 +544,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L38" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:L37">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Buy"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L37"/>
   <sortState ref="A2:L37">
     <sortCondition ref="I1:I37"/>
   </sortState>
@@ -1529,7 +1523,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1577,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1598,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1628,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1658,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1688,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1742,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1766,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1787,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1808,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1829,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1850,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1871,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1892,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1910,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1928,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/ParadigmHyperloop/electrical"
This reverts commit 47d31288c6bddacbab6660df29785a0729d95fbe, reversing
changes made to 90896756f2378821ec6625d68bade529b6c4440f.
</commit_message>
<xml_diff>
--- a/BatteryBoard/bom/bom_pcb.xlsx
+++ b/BatteryBoard/bom/bom_pcb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom_pcb" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L38" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:L37"/>
+  <autoFilter ref="A1:L37">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Buy"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:L37">
     <sortCondition ref="I1:I37"/>
   </sortState>
@@ -1523,7 +1529,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1865,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1922,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Misseed update to BOM
</commit_message>
<xml_diff>
--- a/BatteryBoard/bom/bom_pcb.xlsx
+++ b/BatteryBoard/bom/bom_pcb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="21600" yWindow="460" windowWidth="16800" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom_pcb" sheetId="1" r:id="rId1"/>
@@ -544,13 +544,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L38" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:L37">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Buy"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L37"/>
   <sortState ref="A2:L37">
     <sortCondition ref="I1:I37"/>
   </sortState>
@@ -1529,7 +1523,7 @@
         <v>22.12</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1577,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1598,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1628,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9</v>
       </c>
@@ -1658,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>17</v>
       </c>
@@ -1688,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -1742,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1766,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1787,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1808,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1829,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1850,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1871,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1892,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1910,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1928,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>

</xml_diff>